<commit_message>
Update test results data - 2025-05-12 06:22 PM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 8.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\FBS Result Giver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\DU FBS Mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F90DA7-021F-4284-A858-1DFFC5FE61C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7177ECBC-3243-4A33-A99F-7A5D2CBB2A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1868,15 +1868,15 @@
       </c>
       <c r="AC6" s="20"/>
       <c r="AD6" s="21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AE6">
         <f t="shared" si="13"/>
-        <v>57.5</v>
+        <v>63.5</v>
       </c>
       <c r="AF6">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AH6">
         <f>SUM(AH1:AH5)</f>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="AF11">
         <f t="shared" si="14"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="AF20">
         <f t="shared" si="14"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15" customHeight="1" thickBot="1">

</xml_diff>